<commit_message>
Rendered new version. Removed extra Sankey graphs.
</commit_message>
<xml_diff>
--- a/summary_file_FY2022.xlsx
+++ b/summary_file_FY2022.xlsx
@@ -10040,7 +10040,7 @@
         <v>42</v>
       </c>
       <c r="D548" t="n">
-        <v>19752.11651381</v>
+        <v>19381.02681831</v>
       </c>
       <c r="E548" t="s">
         <v>43</v>
@@ -21937,7 +21937,7 @@
         <v>59</v>
       </c>
       <c r="D696" t="n">
-        <v>1897.14146819</v>
+        <v>1676.31878603</v>
       </c>
       <c r="E696" t="s">
         <v>60</v>
@@ -22447,7 +22447,7 @@
         <v>59</v>
       </c>
       <c r="D726" t="n">
-        <v>1441.10864181</v>
+        <v>1422.1425942</v>
       </c>
       <c r="E726" t="s">
         <v>60</v>
@@ -22566,7 +22566,7 @@
         <v>73</v>
       </c>
       <c r="D733" t="n">
-        <v>2250.39128296</v>
+        <v>1879.30158746</v>
       </c>
       <c r="E733" t="s">
         <v>74</v>
@@ -23020,58 +23020,58 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>106</v>
       </c>
       <c r="B10" t="n">
         <v>2.3</v>
       </c>
       <c r="C10" t="n">
-        <v>34.07</v>
+        <v>4.72</v>
       </c>
       <c r="D10" t="n">
-        <v>7.24</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="B11" t="n">
-        <v>2.3</v>
+        <v>2.1</v>
       </c>
       <c r="C11" t="n">
-        <v>4.72</v>
+        <v>7.21</v>
       </c>
       <c r="D11" t="n">
-        <v>0.44</v>
+        <v>7.54</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="B12" t="n">
-        <v>2.1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>7.21</v>
+        <v>-0.83</v>
       </c>
       <c r="D12" t="n">
-        <v>7.54</v>
+        <v>6.11</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.83</v>
+        <v>11.96</v>
       </c>
       <c r="D13" t="n">
-        <v>6.11</v>
+        <v>6.43</v>
       </c>
     </row>
     <row r="14">
@@ -23124,10 +23124,10 @@
         <v>1.4</v>
       </c>
       <c r="C17" t="n">
-        <v>-24.04</v>
+        <v>-15.16</v>
       </c>
       <c r="D17" t="n">
-        <v>4.83</v>
+        <v>4.77</v>
       </c>
     </row>
     <row r="18">
@@ -23373,13 +23373,13 @@
         <v>43</v>
       </c>
       <c r="B3" t="n">
-        <v>19.8</v>
+        <v>19.4</v>
       </c>
       <c r="C3" t="n">
-        <v>114.47</v>
+        <v>110.44</v>
       </c>
       <c r="D3" t="n">
-        <v>7.17</v>
+        <v>7.09</v>
       </c>
     </row>
     <row r="4">
@@ -23819,22 +23819,22 @@
         <v>43</v>
       </c>
       <c r="B7" t="n">
-        <v>114.47</v>
+        <v>110.44</v>
       </c>
       <c r="C7" t="n">
-        <v>42.66</v>
+        <v>41.31</v>
       </c>
       <c r="D7" t="n">
-        <v>49.24</v>
+        <v>48.3</v>
       </c>
       <c r="E7" t="n">
-        <v>27.19</v>
+        <v>26.71</v>
       </c>
       <c r="F7" t="n">
-        <v>11.91</v>
+        <v>11.69</v>
       </c>
       <c r="G7" t="n">
-        <v>7.17</v>
+        <v>7.09</v>
       </c>
     </row>
     <row r="8">
@@ -24385,22 +24385,22 @@
         <v>60</v>
       </c>
       <c r="B8" t="n">
-        <v>-24.04</v>
+        <v>-15.16</v>
       </c>
       <c r="C8" t="n">
-        <v>52.43</v>
+        <v>51.43</v>
       </c>
       <c r="D8" t="n">
-        <v>35.74</v>
+        <v>35.14</v>
       </c>
       <c r="E8" t="n">
-        <v>17.29</v>
+        <v>16.98</v>
       </c>
       <c r="F8" t="n">
-        <v>3.44</v>
+        <v>3.31</v>
       </c>
       <c r="G8" t="n">
-        <v>4.83</v>
+        <v>4.77</v>
       </c>
     </row>
     <row r="9">
@@ -24822,22 +24822,22 @@
         <v>74</v>
       </c>
       <c r="B27" t="n">
-        <v>34.07</v>
+        <v>11.96</v>
       </c>
       <c r="C27" t="n">
-        <v>41.36</v>
+        <v>29.18</v>
       </c>
       <c r="D27" t="n">
-        <v>55.45</v>
+        <v>46.39</v>
       </c>
       <c r="E27" t="n">
-        <v>35.64</v>
+        <v>30.84</v>
       </c>
       <c r="F27" t="n">
-        <v>16.19</v>
+        <v>14.11</v>
       </c>
       <c r="G27" t="n">
-        <v>7.24</v>
+        <v>6.43</v>
       </c>
     </row>
     <row r="28">
@@ -25287,13 +25287,13 @@
         <v>2021</v>
       </c>
       <c r="B25" t="n">
-        <v>93027.93087085</v>
+        <v>92807.10818869</v>
       </c>
       <c r="C25" t="n">
         <v>91806.06006519</v>
       </c>
       <c r="D25" t="n">
-        <v>-1222</v>
+        <v>-1001</v>
       </c>
     </row>
     <row r="26">
@@ -25301,13 +25301,13 @@
         <v>2022</v>
       </c>
       <c r="B26" t="n">
-        <v>102219.15761718</v>
+        <v>101829.10187407</v>
       </c>
       <c r="C26" t="n">
-        <v>113392.65505891</v>
+        <v>113021.56536341</v>
       </c>
       <c r="D26" t="n">
-        <v>11173</v>
+        <v>11192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>